<commit_message>
UI Changes, Settings Added
</commit_message>
<xml_diff>
--- a/app/src/main/assets/databases/Categories.xlsx
+++ b/app/src/main/assets/databases/Categories.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -144,9 +144,6 @@
     <t>Bodyweight</t>
   </si>
   <si>
-    <t>Bosi</t>
-  </si>
-  <si>
     <t>Battle Rope</t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>TRX</t>
+  </si>
+  <si>
+    <t>Bosu Ball</t>
   </si>
 </sst>
 </file>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF3E0F36-9E64-4617-852E-7022518F5C3D}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,13 +730,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -750,13 +750,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -770,13 +770,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -790,13 +790,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -807,13 +807,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -821,13 +821,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -835,13 +835,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
@@ -849,57 +849,57 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -910,62 +910,62 @@
         <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
         <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -973,12 +973,12 @@
         <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -986,7 +986,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
         <v>27</v>
@@ -997,7 +997,7 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1005,58 +1005,58 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1080,32 +1080,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>